<commit_message>
EPBDS-6773 Impossible to define default values in Datatype for various Java types. All default implemetations were changed to mutable.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test-resources/functionality/Datatype.xlsx
+++ b/DEV/org.openl.test/test-resources/functionality/Datatype.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="20700" windowHeight="11760"/>
+    <workbookView windowHeight="11760" windowWidth="20700" xWindow="480" yWindow="180"/>
   </bookViews>
   <sheets>
-    <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
-    <sheet name="Methods" sheetId="2" r:id="rId2"/>
-    <sheet name="Env" sheetId="3" r:id="rId3"/>
+    <sheet name="Datatypes" r:id="rId1" sheetId="1"/>
+    <sheet name="Methods" r:id="rId2" sheetId="2"/>
+    <sheet name="Env" r:id="rId3" sheetId="3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -21,7 +26,7 @@
     <author>Yury Molchan</author>
   </authors>
   <commentList>
-    <comment ref="D8" authorId="0">
+    <comment authorId="0" ref="D8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0">
+    <comment authorId="0" ref="H8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0">
+    <comment authorId="0" ref="L8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0">
+    <comment authorId="0" ref="P8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0">
+    <comment authorId="0" ref="D41" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H41" authorId="0">
+    <comment authorId="0" ref="H41" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L41" authorId="0">
+    <comment authorId="0" ref="L41" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P41" authorId="0">
+    <comment authorId="0" ref="P41" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -213,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D57" authorId="0">
+    <comment authorId="0" ref="D57" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -237,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H57" authorId="0">
+    <comment authorId="0" ref="H57" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -261,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L57" authorId="0">
+    <comment authorId="0" ref="L57" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -285,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P57" authorId="0">
+    <comment authorId="0" ref="P57" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -309,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D90" authorId="0">
+    <comment authorId="0" ref="D90" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -333,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H90" authorId="0">
+    <comment authorId="0" ref="H90" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -357,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L90" authorId="0">
+    <comment authorId="0" ref="L90" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -381,7 +386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P90" authorId="0">
+    <comment authorId="0" ref="P90" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D106" authorId="0">
+    <comment authorId="0" ref="D106" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -429,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H106" authorId="0">
+    <comment authorId="0" ref="H106" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L106" authorId="0">
+    <comment authorId="0" ref="L106" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -477,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P106" authorId="0">
+    <comment authorId="0" ref="P106" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -501,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D139" authorId="0">
+    <comment authorId="0" ref="D139" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -525,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H139" authorId="0">
+    <comment authorId="0" ref="H139" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -549,7 +554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L139" authorId="0">
+    <comment authorId="0" ref="L139" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -573,7 +578,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="P139" authorId="0">
+    <comment authorId="0" ref="P139" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yury Molchan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Workaround to check all empty values</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="L152" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -602,7 +631,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="294">
   <si>
     <t>Integer</t>
   </si>
@@ -1388,16 +1417,124 @@
   </si>
   <si>
     <t>DoubleValue[][][]</t>
+  </si>
+  <si>
+    <t>Method Boxed getBoxedWithModifiebleCollections()</t>
+  </si>
+  <si>
+    <t>Test getBoxedWithModifiebleCollections boxedWithModifiebleCollectionsTest</t>
+  </si>
+  <si>
+    <t>Boxed ret = new Boxed();
+ret.col.add("value");
+ret.list.add("value");
+ret.map.put("key", "value");
+ret.set.add("value");
+ret.arrayList.add("value");
+ret.hashMap.put("key", "value");
+ret.hashSet.add("value");
+return ret;</t>
+  </si>
+  <si>
+    <t>= new ArrayList().add("value");</t>
+  </si>
+  <si>
+    <t>= new HashMap().put("key","value");</t>
+  </si>
+  <si>
+    <t>= new HashSet().add("value");</t>
+  </si>
+  <si>
+    <t>= new HashMap();</t>
+  </si>
+  <si>
+    <t>= new HashMap().put("key"\,"value");</t>
+  </si>
+  <si>
+    <t>= new HashMap().put("key"/,"value");</t>
+  </si>
+  <si>
+    <t>= new HashMap().put("key"\\,"value");</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>_res_.hashSet</t>
+  </si>
+  <si>
+    <t>_res_.set</t>
+  </si>
+  <si>
+    <t>_res_.arrayList</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>= "value</t>
+  </si>
+  <si>
+    <t>_res_.map</t>
+  </si>
+  <si>
+    <t>= new HashMap().put("key", "value");</t>
+  </si>
+  <si>
+    <t>=value</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>value, value</t>
+  </si>
+  <si>
+    <t>Method Boxed getBoxedWithModifiebleCollectionsTest()</t>
+  </si>
+  <si>
+    <t>Boxed ret = getBoxedWithModifiebleCollections();
+return ret.col.size() + ret.map.size() + ret.set().size() + ret.arrayList.size();</t>
+  </si>
+  <si>
+    <t>Boxed ret = getBoxedWithModifiebleCollections();
+return ret.col.size() + ret.map.size() + ret.set.size() + ret.arrayList.size();</t>
+  </si>
+  <si>
+    <t>Method Integer getBoxedWithModifiebleCollectionsTest()</t>
+  </si>
+  <si>
+    <t>Boxed ret = getBoxedWithModifiebleCollections();
+return ret.col.size() + ret.map.size() + ret.list.size() + ret.set.size() + ret.arrayList.size() + ret.hashSet.size() + ret.hashMap.size();</t>
+  </si>
+  <si>
+    <t>Test getBoxedWithModifiebleCollectionsTest boxedWithModifiebleCollectionsTest</t>
+  </si>
+  <si>
+    <t>_res_.col</t>
+  </si>
+  <si>
+    <t>=_res_</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>res</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="000000" theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1456,7 +1593,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1525,109 +1662,212 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="60">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="8" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="9" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="10" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="11" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="5" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="12" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="4" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1660,9 +1900,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1695,9 +1935,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1730,9 +1987,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1785,7 +2059,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1794,13 +2068,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1810,7 +2084,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1819,7 +2093,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1828,7 +2102,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1838,12 +2112,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1874,7 +2148,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1893,7 +2167,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1905,75 +2179,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P180"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="B3:Q194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I70" sqref="I70"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="L166" sqref="L166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="52.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="15" max="16" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="N3" s="29" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="N3" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="N4" s="30" t="s">
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="N4" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="F7" s="29" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="F7" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="J7" s="31" t="s">
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="J7" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="N7" s="29" t="s">
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="N7" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -1986,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="21" t="str">
-        <f t="shared" ref="F8:F30" si="0">"_res_." &amp; C8</f>
+        <f ref="F8:F30" si="0" t="shared">"_res_." &amp; C8</f>
         <v>_res_.test</v>
       </c>
       <c r="G8" s="1" t="str">
@@ -2006,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="21" t="str">
-        <f t="shared" ref="N8:N30" si="1">"_res_." &amp; K8</f>
+        <f ref="N8:N30" si="1" t="shared">"_res_." &amp; K8</f>
         <v>_res_.test</v>
       </c>
       <c r="O8" s="27" t="str">
@@ -2028,11 +2303,11 @@
         <v>1</v>
       </c>
       <c r="F9" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="G9" s="27" t="str">
-        <f t="shared" ref="G9:G33" si="2">C9</f>
+        <f ref="G9:G33" si="2" t="shared">C9</f>
         <v>byteValue</v>
       </c>
       <c r="H9" s="17">
@@ -2047,11 +2322,11 @@
       </c>
       <c r="L9" s="17"/>
       <c r="N9" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="O9" s="27" t="str">
-        <f t="shared" ref="O9:O33" si="3">K9</f>
+        <f ref="O9:O33" si="3" t="shared">K9</f>
         <v>byteValue</v>
       </c>
       <c r="P9" s="17"/>
@@ -2067,15 +2342,15 @@
         <v>2</v>
       </c>
       <c r="F10" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="G10" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="H10" s="28">
-        <f t="shared" ref="H10:H33" si="4">D10</f>
+        <f ref="H10:H33" si="4" t="shared">D10</f>
         <v>2</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -2086,11 +2361,11 @@
       </c>
       <c r="L10" s="17"/>
       <c r="N10" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="O10" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="P10" s="6"/>
@@ -2106,15 +2381,15 @@
         <v>3</v>
       </c>
       <c r="F11" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="G11" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="H11" s="28">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>3</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -2125,11 +2400,11 @@
       </c>
       <c r="L11" s="17"/>
       <c r="N11" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="O11" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="P11" s="6"/>
@@ -2145,15 +2420,15 @@
         <v>4</v>
       </c>
       <c r="F12" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="G12" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="H12" s="28">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>4</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -2164,11 +2439,11 @@
       </c>
       <c r="L12" s="17"/>
       <c r="N12" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="O12" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="P12" s="6"/>
@@ -2184,15 +2459,15 @@
         <v>5</v>
       </c>
       <c r="F13" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="G13" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="H13" s="28">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>5</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -2203,11 +2478,11 @@
       </c>
       <c r="L13" s="17"/>
       <c r="N13" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="O13" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="P13" s="6"/>
@@ -2223,15 +2498,15 @@
         <v>6</v>
       </c>
       <c r="F14" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="G14" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="H14" s="28">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>6</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -2242,11 +2517,11 @@
       </c>
       <c r="L14" s="17"/>
       <c r="N14" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="O14" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="P14" s="6"/>
@@ -2262,15 +2537,15 @@
         <v>19</v>
       </c>
       <c r="F15" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="G15" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="H15" s="28" t="str">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>y</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -2281,11 +2556,11 @@
       </c>
       <c r="L15" s="17"/>
       <c r="N15" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="O15" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="P15" s="6"/>
@@ -2301,15 +2576,15 @@
         <v>114</v>
       </c>
       <c r="F16" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="G16" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="H16" s="28" t="str">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>A</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -2320,11 +2595,11 @@
       </c>
       <c r="L16" s="17"/>
       <c r="N16" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="O16" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="P16" s="6"/>
@@ -2340,15 +2615,15 @@
         <v>20</v>
       </c>
       <c r="F17" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.string</v>
       </c>
       <c r="G17" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>string</v>
       </c>
       <c r="H17" s="28" t="str">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>str</v>
       </c>
       <c r="J17" s="1" t="s">
@@ -2359,11 +2634,11 @@
       </c>
       <c r="L17" s="17"/>
       <c r="N17" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.stringValue</v>
       </c>
       <c r="O17" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>stringValue</v>
       </c>
       <c r="P17" s="6"/>
@@ -2379,15 +2654,15 @@
         <v>95</v>
       </c>
       <c r="F18" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.date</v>
       </c>
       <c r="G18" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>date</v>
       </c>
       <c r="H18" s="28" t="str">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>03/31/2017</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -2398,11 +2673,11 @@
       </c>
       <c r="L18" s="2"/>
       <c r="N18" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.dateValue</v>
       </c>
       <c r="O18" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>dateValue</v>
       </c>
       <c r="P18" s="2"/>
@@ -2418,15 +2693,15 @@
         <v>7</v>
       </c>
       <c r="F19" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.bigInt</v>
       </c>
       <c r="G19" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>bigInt</v>
       </c>
       <c r="H19" s="28">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>7</v>
       </c>
       <c r="J19" s="1" t="s">
@@ -2437,11 +2712,11 @@
       </c>
       <c r="L19" s="17"/>
       <c r="N19" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.bigIntValue</v>
       </c>
       <c r="O19" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>bigIntValue</v>
       </c>
       <c r="P19" s="6"/>
@@ -2457,15 +2732,15 @@
         <v>8</v>
       </c>
       <c r="F20" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.bigDec</v>
       </c>
       <c r="G20" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>bigDec</v>
       </c>
       <c r="H20" s="28">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>8</v>
       </c>
       <c r="J20" s="1" t="s">
@@ -2476,11 +2751,11 @@
       </c>
       <c r="L20" s="17"/>
       <c r="N20" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.bigDecValue</v>
       </c>
       <c r="O20" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>bigDecValue</v>
       </c>
       <c r="P20" s="6"/>
@@ -2496,11 +2771,11 @@
         <v>2</v>
       </c>
       <c r="F21" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.col</v>
       </c>
       <c r="G21" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>col</v>
       </c>
       <c r="H21" s="28"/>
@@ -2512,11 +2787,11 @@
       </c>
       <c r="L21" s="17"/>
       <c r="N21" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.colValue</v>
       </c>
       <c r="O21" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>colValue</v>
       </c>
       <c r="P21" s="10"/>
@@ -2532,11 +2807,11 @@
         <v>2</v>
       </c>
       <c r="F22" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.list</v>
       </c>
       <c r="G22" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>list</v>
       </c>
       <c r="H22" s="28"/>
@@ -2548,11 +2823,11 @@
       </c>
       <c r="L22" s="17"/>
       <c r="N22" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.listValue</v>
       </c>
       <c r="O22" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>listValue</v>
       </c>
       <c r="P22" s="6"/>
@@ -2568,11 +2843,11 @@
         <v>2</v>
       </c>
       <c r="F23" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.map</v>
       </c>
       <c r="G23" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>map</v>
       </c>
       <c r="H23" s="28"/>
@@ -2584,11 +2859,11 @@
       </c>
       <c r="L23" s="17"/>
       <c r="N23" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.mapValue</v>
       </c>
       <c r="O23" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>mapValue</v>
       </c>
       <c r="P23" s="6"/>
@@ -2604,11 +2879,11 @@
         <v>2</v>
       </c>
       <c r="F24" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.set</v>
       </c>
       <c r="G24" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>set</v>
       </c>
       <c r="H24" s="28"/>
@@ -2620,11 +2895,11 @@
       </c>
       <c r="L24" s="17"/>
       <c r="N24" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.setValue</v>
       </c>
       <c r="O24" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>setValue</v>
       </c>
       <c r="P24" s="6"/>
@@ -2640,11 +2915,11 @@
         <v>2</v>
       </c>
       <c r="F25" s="21" t="str">
-        <f t="shared" ref="F25:F28" si="5">"_res_." &amp; C25</f>
+        <f ref="F25:F28" si="5" t="shared">"_res_." &amp; C25</f>
         <v>_res_.arrayList</v>
       </c>
       <c r="G25" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>arrayList</v>
       </c>
       <c r="H25" s="28"/>
@@ -2656,11 +2931,11 @@
       </c>
       <c r="L25" s="21"/>
       <c r="N25" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.arrayList</v>
       </c>
       <c r="O25" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>arrayList</v>
       </c>
       <c r="P25" s="21"/>
@@ -2676,11 +2951,11 @@
         <v>2</v>
       </c>
       <c r="F26" s="21" t="str">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>_res_.hashMap</v>
       </c>
       <c r="G26" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>hashMap</v>
       </c>
       <c r="H26" s="28"/>
@@ -2692,11 +2967,11 @@
       </c>
       <c r="L26" s="21"/>
       <c r="N26" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.hashMap</v>
       </c>
       <c r="O26" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>hashMap</v>
       </c>
       <c r="P26" s="21"/>
@@ -2712,11 +2987,11 @@
         <v>2</v>
       </c>
       <c r="F27" s="21" t="str">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>_res_.hashSet</v>
       </c>
       <c r="G27" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>hashSet</v>
       </c>
       <c r="H27" s="28"/>
@@ -2728,11 +3003,11 @@
       </c>
       <c r="L27" s="21"/>
       <c r="N27" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.hashSet</v>
       </c>
       <c r="O27" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>hashSet</v>
       </c>
       <c r="P27" s="21"/>
@@ -2748,15 +3023,15 @@
         <v>242</v>
       </c>
       <c r="F28" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>_res_.gender</v>
       </c>
       <c r="G28" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>gender</v>
       </c>
       <c r="H28" s="28" t="str">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>Male</v>
       </c>
       <c r="J28" s="22" t="s">
@@ -2767,11 +3042,11 @@
       </c>
       <c r="L28" s="22"/>
       <c r="N28" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.gender</v>
       </c>
       <c r="O28" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>gender</v>
       </c>
       <c r="P28" s="22"/>
@@ -2787,11 +3062,11 @@
         <v>2</v>
       </c>
       <c r="F29" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.address</v>
       </c>
       <c r="G29" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>address</v>
       </c>
       <c r="H29" s="28"/>
@@ -2803,11 +3078,11 @@
       </c>
       <c r="L29" s="20"/>
       <c r="N29" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.address</v>
       </c>
       <c r="O29" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>address</v>
       </c>
       <c r="P29" s="20"/>
@@ -2823,11 +3098,11 @@
         <v>2</v>
       </c>
       <c r="F30" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>_res_.person</v>
       </c>
       <c r="G30" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>person</v>
       </c>
       <c r="H30" s="28"/>
@@ -2839,11 +3114,11 @@
       </c>
       <c r="L30" s="20"/>
       <c r="N30" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>_res_.person</v>
       </c>
       <c r="O30" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>person</v>
       </c>
       <c r="P30" s="20"/>
@@ -2863,7 +3138,7 @@
         <v>_res_.auto</v>
       </c>
       <c r="G31" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>auto</v>
       </c>
       <c r="H31" s="28"/>
@@ -2879,7 +3154,7 @@
         <v>_res_.auto</v>
       </c>
       <c r="O31" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>auto</v>
       </c>
       <c r="P31" s="20"/>
@@ -2899,11 +3174,11 @@
         <v>_res_.roudingMode</v>
       </c>
       <c r="G32" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>roudingMode</v>
       </c>
       <c r="H32" s="28" t="str">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>HALF_EVEN</v>
       </c>
       <c r="J32" s="24" t="s">
@@ -2918,7 +3193,7 @@
         <v>_res_.roudingMode</v>
       </c>
       <c r="O32" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>roudingMode</v>
       </c>
       <c r="P32" s="24"/>
@@ -2938,11 +3213,11 @@
         <v>_res_.dv</v>
       </c>
       <c r="G33" s="27" t="str">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>dv</v>
       </c>
       <c r="H33" s="28">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>10.1</v>
       </c>
       <c r="J33" s="26" t="s">
@@ -2957,56 +3232,56 @@
         <v>_res_.dv</v>
       </c>
       <c r="O33" s="27" t="str">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>dv</v>
       </c>
       <c r="P33" s="26"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F36" s="29" t="s">
+      <c r="F36" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="N36" s="29" t="s">
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="N36" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="O36" s="29"/>
-      <c r="P36" s="29"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="31"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F37" s="30" t="s">
+      <c r="F37" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="N37" s="30" t="s">
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="N37" s="41" t="s">
         <v>139</v>
       </c>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="41"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="F40" s="33" t="s">
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="F40" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="J40" s="31" t="s">
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="J40" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="N40" s="33" t="s">
+      <c r="K40" s="42"/>
+      <c r="L40" s="42"/>
+      <c r="N40" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
+      <c r="O40" s="44"/>
+      <c r="P40" s="44"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="17" t="s">
@@ -3019,7 +3294,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="21" t="str">
-        <f t="shared" ref="F41:F49" si="6">"_res_." &amp; C41</f>
+        <f ref="F41:F49" si="6" t="shared">"_res_." &amp; C41</f>
         <v>_res_.test</v>
       </c>
       <c r="G41" s="17" t="str">
@@ -3039,7 +3314,7 @@
         <v>1</v>
       </c>
       <c r="N41" s="21" t="str">
-        <f t="shared" ref="N41:N49" si="7">"_res_." &amp; K41</f>
+        <f ref="N41:N49" si="7" t="shared">"_res_." &amp; K41</f>
         <v>_res_.test</v>
       </c>
       <c r="O41" s="27" t="str">
@@ -3061,11 +3336,11 @@
         <v>1</v>
       </c>
       <c r="F42" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="G42" s="27" t="str">
-        <f t="shared" ref="G42:G49" si="8">C42</f>
+        <f ref="G42:G49" si="8" t="shared">C42</f>
         <v>byteValue</v>
       </c>
       <c r="H42" s="1">
@@ -3080,11 +3355,11 @@
       </c>
       <c r="L42" s="17"/>
       <c r="N42" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="O42" s="27" t="str">
-        <f t="shared" ref="O42:O49" si="9">K42</f>
+        <f ref="O42:O49" si="9" t="shared">K42</f>
         <v>byteValue</v>
       </c>
       <c r="P42" s="6">
@@ -3102,15 +3377,15 @@
         <v>2</v>
       </c>
       <c r="F43" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="G43" s="27" t="str">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="H43" s="28">
-        <f t="shared" ref="H43:H49" si="10">D43</f>
+        <f ref="H43:H49" si="10" t="shared">D43</f>
         <v>2</v>
       </c>
       <c r="J43" s="6" t="s">
@@ -3121,11 +3396,11 @@
       </c>
       <c r="L43" s="17"/>
       <c r="N43" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="O43" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="P43" s="6">
@@ -3143,15 +3418,15 @@
         <v>3</v>
       </c>
       <c r="F44" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="G44" s="27" t="str">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="H44" s="28">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>3</v>
       </c>
       <c r="J44" s="6" t="s">
@@ -3162,11 +3437,11 @@
       </c>
       <c r="L44" s="17"/>
       <c r="N44" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="O44" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="P44" s="6">
@@ -3184,15 +3459,15 @@
         <v>4</v>
       </c>
       <c r="F45" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="G45" s="27" t="str">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="H45" s="28">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>4</v>
       </c>
       <c r="J45" s="6" t="s">
@@ -3203,11 +3478,11 @@
       </c>
       <c r="L45" s="17"/>
       <c r="N45" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="O45" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="P45" s="6">
@@ -3225,15 +3500,15 @@
         <v>5</v>
       </c>
       <c r="F46" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="G46" s="27" t="str">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="H46" s="28">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>5</v>
       </c>
       <c r="J46" s="6" t="s">
@@ -3244,11 +3519,11 @@
       </c>
       <c r="L46" s="17"/>
       <c r="N46" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="O46" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="P46" s="6">
@@ -3266,15 +3541,15 @@
         <v>6</v>
       </c>
       <c r="F47" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="G47" s="27" t="str">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="H47" s="28">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>6</v>
       </c>
       <c r="J47" s="6" t="s">
@@ -3285,11 +3560,11 @@
       </c>
       <c r="L47" s="17"/>
       <c r="N47" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="O47" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="P47" s="6">
@@ -3307,15 +3582,15 @@
         <v>19</v>
       </c>
       <c r="F48" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="G48" s="27" t="str">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="H48" s="28" t="str">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>y</v>
       </c>
       <c r="J48" s="6" t="s">
@@ -3326,11 +3601,11 @@
       </c>
       <c r="L48" s="17"/>
       <c r="N48" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="O48" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="P48" s="6" t="b">
@@ -3348,15 +3623,15 @@
         <v>114</v>
       </c>
       <c r="F49" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="G49" s="27" t="str">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="H49" s="28" t="str">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>A</v>
       </c>
       <c r="J49" s="1" t="s">
@@ -3367,60 +3642,60 @@
       </c>
       <c r="L49" s="17"/>
       <c r="N49" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="O49" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="P49" s="6"/>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F52" s="29" t="s">
+      <c r="F52" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29"/>
-      <c r="N52" s="29" t="s">
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="N52" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="O52" s="29"/>
-      <c r="P52" s="29"/>
+      <c r="O52" s="31"/>
+      <c r="P52" s="31"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F53" s="30" t="s">
+      <c r="F53" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
-      <c r="N53" s="30" t="s">
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="N53" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="O53" s="30"/>
-      <c r="P53" s="30"/>
+      <c r="O53" s="41"/>
+      <c r="P53" s="41"/>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B56" s="29" t="s">
+      <c r="B56" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="F56" s="29" t="s">
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="F56" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="G56" s="29"/>
-      <c r="H56" s="29"/>
-      <c r="J56" s="31" t="s">
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="J56" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="K56" s="31"/>
-      <c r="L56" s="31"/>
-      <c r="N56" s="29" t="s">
+      <c r="K56" s="42"/>
+      <c r="L56" s="42"/>
+      <c r="N56" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="O56" s="29"/>
-      <c r="P56" s="29"/>
+      <c r="O56" s="31"/>
+      <c r="P56" s="31"/>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" s="17" t="s">
@@ -3433,7 +3708,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="21" t="str">
-        <f t="shared" ref="F57:F80" si="11">"_res_." &amp; C57</f>
+        <f ref="F57:F80" si="11" t="shared">"_res_." &amp; C57</f>
         <v>_res_.test</v>
       </c>
       <c r="G57" s="17" t="str">
@@ -3453,7 +3728,7 @@
         <v>1</v>
       </c>
       <c r="N57" s="21" t="str">
-        <f t="shared" ref="N57:N80" si="12">"_res_." &amp; K57</f>
+        <f ref="N57:N80" si="12" t="shared">"_res_." &amp; K57</f>
         <v>_res_.test</v>
       </c>
       <c r="O57" s="27" t="str">
@@ -3475,7 +3750,7 @@
         <v>55</v>
       </c>
       <c r="F58" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="G58" s="27" t="str">
@@ -3494,11 +3769,11 @@
       </c>
       <c r="L58" s="17"/>
       <c r="N58" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="O58" s="27" t="str">
-        <f t="shared" ref="O58:O82" si="13">K58</f>
+        <f ref="O58:O82" si="13" t="shared">K58</f>
         <v>byteValue</v>
       </c>
       <c r="P58" s="12"/>
@@ -3514,15 +3789,15 @@
         <v>55</v>
       </c>
       <c r="F59" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="G59" s="27" t="str">
-        <f t="shared" ref="G59:G82" si="14">C59</f>
+        <f ref="G59:G82" si="14" t="shared">C59</f>
         <v>shortValue</v>
       </c>
       <c r="H59" s="28" t="str">
-        <f t="shared" ref="H59:H82" si="15">D59</f>
+        <f ref="H59:H82" si="15" t="shared">D59</f>
         <v>1,2,3</v>
       </c>
       <c r="J59" s="1" t="s">
@@ -3533,11 +3808,11 @@
       </c>
       <c r="L59" s="17"/>
       <c r="N59" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="O59" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="P59" s="12"/>
@@ -3553,15 +3828,15 @@
         <v>55</v>
       </c>
       <c r="F60" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="G60" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="H60" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>1,2,3</v>
       </c>
       <c r="J60" s="1" t="s">
@@ -3572,11 +3847,11 @@
       </c>
       <c r="L60" s="17"/>
       <c r="N60" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="O60" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="P60" s="12"/>
@@ -3592,15 +3867,15 @@
         <v>55</v>
       </c>
       <c r="F61" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="G61" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="H61" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>1,2,3</v>
       </c>
       <c r="J61" s="1" t="s">
@@ -3611,11 +3886,11 @@
       </c>
       <c r="L61" s="17"/>
       <c r="N61" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="O61" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="P61" s="12"/>
@@ -3631,15 +3906,15 @@
         <v>55</v>
       </c>
       <c r="F62" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="G62" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="H62" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>1,2,3</v>
       </c>
       <c r="J62" s="1" t="s">
@@ -3650,11 +3925,11 @@
       </c>
       <c r="L62" s="17"/>
       <c r="N62" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="O62" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="P62" s="12"/>
@@ -3670,15 +3945,15 @@
         <v>55</v>
       </c>
       <c r="F63" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="G63" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="H63" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>1,2,3</v>
       </c>
       <c r="J63" s="1" t="s">
@@ -3689,11 +3964,11 @@
       </c>
       <c r="L63" s="17"/>
       <c r="N63" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="O63" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="P63" s="12"/>
@@ -3709,15 +3984,15 @@
         <v>56</v>
       </c>
       <c r="F64" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="G64" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="H64" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>y,n</v>
       </c>
       <c r="J64" s="1" t="s">
@@ -3728,11 +4003,11 @@
       </c>
       <c r="L64" s="17"/>
       <c r="N64" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="O64" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="P64" s="12"/>
@@ -3748,15 +4023,15 @@
         <v>57</v>
       </c>
       <c r="F65" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="G65" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="H65" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>A,B,C</v>
       </c>
       <c r="J65" s="1" t="s">
@@ -3767,11 +4042,11 @@
       </c>
       <c r="L65" s="17"/>
       <c r="N65" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="O65" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="P65" s="12"/>
@@ -3787,15 +4062,15 @@
         <v>62</v>
       </c>
       <c r="F66" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.stringValue</v>
       </c>
       <c r="G66" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>stringValue</v>
       </c>
       <c r="H66" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>str1, str2</v>
       </c>
       <c r="J66" s="1" t="s">
@@ -3806,11 +4081,11 @@
       </c>
       <c r="L66" s="17"/>
       <c r="N66" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.stringValue</v>
       </c>
       <c r="O66" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>stringValue</v>
       </c>
       <c r="P66" s="12"/>
@@ -3826,15 +4101,15 @@
         <v>95</v>
       </c>
       <c r="F67" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.dateValue</v>
       </c>
       <c r="G67" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>dateValue</v>
       </c>
       <c r="H67" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>03/31/2017</v>
       </c>
       <c r="J67" s="1" t="s">
@@ -3845,11 +4120,11 @@
       </c>
       <c r="L67" s="2"/>
       <c r="N67" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.dateValue</v>
       </c>
       <c r="O67" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>dateValue</v>
       </c>
       <c r="P67" s="2"/>
@@ -3865,15 +4140,15 @@
         <v>55</v>
       </c>
       <c r="F68" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.bigIntValue</v>
       </c>
       <c r="G68" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>bigIntValue</v>
       </c>
       <c r="H68" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>1,2,3</v>
       </c>
       <c r="J68" s="1" t="s">
@@ -3884,11 +4159,11 @@
       </c>
       <c r="L68" s="17"/>
       <c r="N68" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.bigIntValue</v>
       </c>
       <c r="O68" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>bigIntValue</v>
       </c>
       <c r="P68" s="12"/>
@@ -3904,15 +4179,15 @@
         <v>55</v>
       </c>
       <c r="F69" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.bigDecValue</v>
       </c>
       <c r="G69" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>bigDecValue</v>
       </c>
       <c r="H69" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>1,2,3</v>
       </c>
       <c r="J69" s="1" t="s">
@@ -3923,11 +4198,11 @@
       </c>
       <c r="L69" s="17"/>
       <c r="N69" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.bigDecValue</v>
       </c>
       <c r="O69" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>bigDecValue</v>
       </c>
       <c r="P69" s="12"/>
@@ -3943,11 +4218,11 @@
         <v>2</v>
       </c>
       <c r="F70" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.colValue</v>
       </c>
       <c r="G70" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>colValue</v>
       </c>
       <c r="H70" s="28"/>
@@ -3959,11 +4234,11 @@
       </c>
       <c r="L70" s="17"/>
       <c r="N70" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.colValue</v>
       </c>
       <c r="O70" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>colValue</v>
       </c>
       <c r="P70" s="12"/>
@@ -3979,11 +4254,11 @@
         <v>2</v>
       </c>
       <c r="F71" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.listValue</v>
       </c>
       <c r="G71" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>listValue</v>
       </c>
       <c r="H71" s="28"/>
@@ -3995,11 +4270,11 @@
       </c>
       <c r="L71" s="17"/>
       <c r="N71" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.listValue</v>
       </c>
       <c r="O71" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>listValue</v>
       </c>
       <c r="P71" s="12"/>
@@ -4015,11 +4290,11 @@
         <v>2</v>
       </c>
       <c r="F72" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.mapValue</v>
       </c>
       <c r="G72" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>mapValue</v>
       </c>
       <c r="H72" s="28"/>
@@ -4031,11 +4306,11 @@
       </c>
       <c r="L72" s="17"/>
       <c r="N72" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.mapValue</v>
       </c>
       <c r="O72" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>mapValue</v>
       </c>
       <c r="P72" s="12"/>
@@ -4051,11 +4326,11 @@
         <v>2</v>
       </c>
       <c r="F73" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.setValue</v>
       </c>
       <c r="G73" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>setValue</v>
       </c>
       <c r="H73" s="28"/>
@@ -4067,11 +4342,11 @@
       </c>
       <c r="L73" s="17"/>
       <c r="N73" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.setValue</v>
       </c>
       <c r="O73" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>setValue</v>
       </c>
       <c r="P73" s="12"/>
@@ -4087,11 +4362,11 @@
         <v>2</v>
       </c>
       <c r="F74" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.arrayList</v>
       </c>
       <c r="G74" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>arrayList</v>
       </c>
       <c r="H74" s="28"/>
@@ -4103,11 +4378,11 @@
       </c>
       <c r="L74" s="21"/>
       <c r="N74" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.arrayList</v>
       </c>
       <c r="O74" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>arrayList</v>
       </c>
       <c r="P74" s="21"/>
@@ -4123,11 +4398,11 @@
         <v>2</v>
       </c>
       <c r="F75" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.hashMap</v>
       </c>
       <c r="G75" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>hashMap</v>
       </c>
       <c r="H75" s="28"/>
@@ -4139,11 +4414,11 @@
       </c>
       <c r="L75" s="21"/>
       <c r="N75" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.hashMap</v>
       </c>
       <c r="O75" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>hashMap</v>
       </c>
       <c r="P75" s="21"/>
@@ -4159,11 +4434,11 @@
         <v>2</v>
       </c>
       <c r="F76" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.hashSet</v>
       </c>
       <c r="G76" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>hashSet</v>
       </c>
       <c r="H76" s="28"/>
@@ -4175,11 +4450,11 @@
       </c>
       <c r="L76" s="21"/>
       <c r="N76" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.hashSet</v>
       </c>
       <c r="O76" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>hashSet</v>
       </c>
       <c r="P76" s="21"/>
@@ -4195,15 +4470,15 @@
         <v>249</v>
       </c>
       <c r="F77" s="22" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.gender</v>
       </c>
       <c r="G77" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>gender</v>
       </c>
       <c r="H77" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>Male, Female</v>
       </c>
       <c r="J77" s="22" t="s">
@@ -4214,11 +4489,11 @@
       </c>
       <c r="L77" s="22"/>
       <c r="N77" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.gender</v>
       </c>
       <c r="O77" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>gender</v>
       </c>
       <c r="P77" s="22"/>
@@ -4234,11 +4509,11 @@
         <v>2</v>
       </c>
       <c r="F78" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.address</v>
       </c>
       <c r="G78" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>address</v>
       </c>
       <c r="H78" s="28"/>
@@ -4250,11 +4525,11 @@
       </c>
       <c r="L78" s="20"/>
       <c r="N78" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.address</v>
       </c>
       <c r="O78" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>address</v>
       </c>
       <c r="P78" s="20"/>
@@ -4270,11 +4545,11 @@
         <v>2</v>
       </c>
       <c r="F79" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.person</v>
       </c>
       <c r="G79" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>person</v>
       </c>
       <c r="H79" s="28"/>
@@ -4286,11 +4561,11 @@
       </c>
       <c r="L79" s="20"/>
       <c r="N79" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.person</v>
       </c>
       <c r="O79" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>person</v>
       </c>
       <c r="P79" s="20"/>
@@ -4306,11 +4581,11 @@
         <v>2</v>
       </c>
       <c r="F80" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>_res_.auto</v>
       </c>
       <c r="G80" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>auto</v>
       </c>
       <c r="H80" s="28"/>
@@ -4322,11 +4597,11 @@
       </c>
       <c r="L80" s="20"/>
       <c r="N80" s="21" t="str">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>_res_.auto</v>
       </c>
       <c r="O80" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>auto</v>
       </c>
       <c r="P80" s="20"/>
@@ -4346,11 +4621,11 @@
         <v>_res_.roudingMode</v>
       </c>
       <c r="G81" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>roudingMode</v>
       </c>
       <c r="H81" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>UP, DOWN</v>
       </c>
       <c r="J81" s="25" t="s">
@@ -4365,7 +4640,7 @@
         <v>_res_.roudingMode</v>
       </c>
       <c r="O81" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>roudingMode</v>
       </c>
       <c r="P81" s="25"/>
@@ -4385,11 +4660,11 @@
         <v>_res_.dv</v>
       </c>
       <c r="G82" s="27" t="str">
-        <f t="shared" si="14"/>
+        <f si="14" t="shared"/>
         <v>dv</v>
       </c>
       <c r="H82" s="28" t="str">
-        <f t="shared" si="15"/>
+        <f si="15" t="shared"/>
         <v>10.1, 22.4</v>
       </c>
       <c r="J82" s="26" t="s">
@@ -4404,56 +4679,56 @@
         <v>_res_.dv</v>
       </c>
       <c r="O82" s="27" t="str">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>dv</v>
       </c>
       <c r="P82" s="26"/>
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F85" s="29" t="s">
+      <c r="F85" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="G85" s="29"/>
-      <c r="H85" s="29"/>
-      <c r="N85" s="29" t="s">
+      <c r="G85" s="31"/>
+      <c r="H85" s="31"/>
+      <c r="N85" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="O85" s="29"/>
-      <c r="P85" s="29"/>
+      <c r="O85" s="31"/>
+      <c r="P85" s="31"/>
     </row>
     <row r="86" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F86" s="30" t="s">
+      <c r="F86" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="G86" s="30"/>
-      <c r="H86" s="30"/>
-      <c r="N86" s="30" t="s">
+      <c r="G86" s="41"/>
+      <c r="H86" s="41"/>
+      <c r="N86" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="O86" s="30"/>
-      <c r="P86" s="30"/>
+      <c r="O86" s="41"/>
+      <c r="P86" s="41"/>
     </row>
     <row r="89" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B89" s="32" t="s">
+      <c r="B89" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C89" s="32"/>
-      <c r="D89" s="32"/>
-      <c r="F89" s="29" t="s">
+      <c r="C89" s="43"/>
+      <c r="D89" s="43"/>
+      <c r="F89" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="G89" s="29"/>
-      <c r="H89" s="29"/>
-      <c r="J89" s="31" t="s">
+      <c r="G89" s="31"/>
+      <c r="H89" s="31"/>
+      <c r="J89" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="K89" s="31"/>
-      <c r="L89" s="31"/>
-      <c r="N89" s="33" t="s">
+      <c r="K89" s="42"/>
+      <c r="L89" s="42"/>
+      <c r="N89" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="O89" s="33"/>
-      <c r="P89" s="33"/>
+      <c r="O89" s="44"/>
+      <c r="P89" s="44"/>
     </row>
     <row r="90" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B90" s="17" t="s">
@@ -4466,11 +4741,11 @@
         <v>1</v>
       </c>
       <c r="F90" s="21" t="str">
-        <f t="shared" ref="F90:F98" si="16">"_res_." &amp; C90</f>
+        <f ref="F90:F98" si="16" t="shared">"_res_." &amp; C90</f>
         <v>_res_.test</v>
       </c>
       <c r="G90" s="27" t="str">
-        <f t="shared" ref="G90:G98" si="17">C90</f>
+        <f ref="G90:G98" si="17" t="shared">C90</f>
         <v>test</v>
       </c>
       <c r="H90" s="17">
@@ -4486,11 +4761,11 @@
         <v>1</v>
       </c>
       <c r="N90" s="21" t="str">
-        <f t="shared" ref="N90:N98" si="18">"_res_." &amp; K90</f>
+        <f ref="N90:N98" si="18" t="shared">"_res_." &amp; K90</f>
         <v>_res_.test</v>
       </c>
       <c r="O90" s="27" t="str">
-        <f t="shared" ref="O90:O98" si="19">K90</f>
+        <f ref="O90:O98" si="19" t="shared">K90</f>
         <v>test</v>
       </c>
       <c r="P90" s="17">
@@ -4508,11 +4783,11 @@
         <v>55</v>
       </c>
       <c r="F91" s="21" t="str">
-        <f t="shared" si="16"/>
+        <f si="16" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="G91" s="27" t="str">
-        <f t="shared" si="17"/>
+        <f si="17" t="shared"/>
         <v>byteValue</v>
       </c>
       <c r="H91" s="13" t="s">
@@ -4526,11 +4801,11 @@
       </c>
       <c r="L91" s="17"/>
       <c r="N91" s="21" t="str">
-        <f t="shared" si="18"/>
+        <f si="18" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="O91" s="27" t="str">
-        <f t="shared" si="19"/>
+        <f si="19" t="shared"/>
         <v>byteValue</v>
       </c>
       <c r="P91" s="13"/>
@@ -4546,11 +4821,11 @@
         <v>55</v>
       </c>
       <c r="F92" s="21" t="str">
-        <f t="shared" si="16"/>
+        <f si="16" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="G92" s="27" t="str">
-        <f t="shared" si="17"/>
+        <f si="17" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="H92" s="13" t="s">
@@ -4564,11 +4839,11 @@
       </c>
       <c r="L92" s="17"/>
       <c r="N92" s="21" t="str">
-        <f t="shared" si="18"/>
+        <f si="18" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="O92" s="27" t="str">
-        <f t="shared" si="19"/>
+        <f si="19" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="P92" s="13"/>
@@ -4584,11 +4859,11 @@
         <v>55</v>
       </c>
       <c r="F93" s="21" t="str">
-        <f t="shared" si="16"/>
+        <f si="16" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="G93" s="27" t="str">
-        <f t="shared" si="17"/>
+        <f si="17" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="H93" s="13" t="s">
@@ -4602,11 +4877,11 @@
       </c>
       <c r="L93" s="17"/>
       <c r="N93" s="21" t="str">
-        <f t="shared" si="18"/>
+        <f si="18" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="O93" s="27" t="str">
-        <f t="shared" si="19"/>
+        <f si="19" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="P93" s="13"/>
@@ -4622,11 +4897,11 @@
         <v>55</v>
       </c>
       <c r="F94" s="21" t="str">
-        <f t="shared" si="16"/>
+        <f si="16" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="G94" s="27" t="str">
-        <f t="shared" si="17"/>
+        <f si="17" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="H94" s="13" t="s">
@@ -4640,11 +4915,11 @@
       </c>
       <c r="L94" s="17"/>
       <c r="N94" s="21" t="str">
-        <f t="shared" si="18"/>
+        <f si="18" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="O94" s="27" t="str">
-        <f t="shared" si="19"/>
+        <f si="19" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="P94" s="13"/>
@@ -4660,11 +4935,11 @@
         <v>55</v>
       </c>
       <c r="F95" s="21" t="str">
-        <f t="shared" si="16"/>
+        <f si="16" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="G95" s="27" t="str">
-        <f t="shared" si="17"/>
+        <f si="17" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="H95" s="13" t="s">
@@ -4678,11 +4953,11 @@
       </c>
       <c r="L95" s="17"/>
       <c r="N95" s="21" t="str">
-        <f t="shared" si="18"/>
+        <f si="18" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="O95" s="27" t="str">
-        <f t="shared" si="19"/>
+        <f si="19" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="P95" s="13"/>
@@ -4698,11 +4973,11 @@
         <v>55</v>
       </c>
       <c r="F96" s="21" t="str">
-        <f t="shared" si="16"/>
+        <f si="16" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="G96" s="27" t="str">
-        <f t="shared" si="17"/>
+        <f si="17" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="H96" s="13" t="s">
@@ -4716,11 +4991,11 @@
       </c>
       <c r="L96" s="17"/>
       <c r="N96" s="21" t="str">
-        <f t="shared" si="18"/>
+        <f si="18" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="O96" s="27" t="str">
-        <f t="shared" si="19"/>
+        <f si="19" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="P96" s="13"/>
@@ -4736,11 +5011,11 @@
         <v>56</v>
       </c>
       <c r="F97" s="21" t="str">
-        <f t="shared" si="16"/>
+        <f si="16" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="G97" s="27" t="str">
-        <f t="shared" si="17"/>
+        <f si="17" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="H97" s="13" t="s">
@@ -4754,11 +5029,11 @@
       </c>
       <c r="L97" s="17"/>
       <c r="N97" s="21" t="str">
-        <f t="shared" si="18"/>
+        <f si="18" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="O97" s="27" t="str">
-        <f t="shared" si="19"/>
+        <f si="19" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="P97" s="13"/>
@@ -4774,11 +5049,11 @@
         <v>57</v>
       </c>
       <c r="F98" s="21" t="str">
-        <f t="shared" si="16"/>
+        <f si="16" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="G98" s="27" t="str">
-        <f t="shared" si="17"/>
+        <f si="17" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="H98" s="13" t="s">
@@ -4792,60 +5067,60 @@
       </c>
       <c r="L98" s="17"/>
       <c r="N98" s="21" t="str">
-        <f t="shared" si="18"/>
+        <f si="18" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="O98" s="27" t="str">
-        <f t="shared" si="19"/>
+        <f si="19" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="P98" s="13"/>
     </row>
     <row r="101" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F101" s="29" t="s">
+      <c r="F101" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="G101" s="29"/>
-      <c r="H101" s="29"/>
-      <c r="N101" s="29" t="s">
+      <c r="G101" s="31"/>
+      <c r="H101" s="31"/>
+      <c r="N101" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="O101" s="29"/>
-      <c r="P101" s="29"/>
+      <c r="O101" s="31"/>
+      <c r="P101" s="31"/>
     </row>
     <row r="102" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F102" s="30" t="s">
+      <c r="F102" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="G102" s="30"/>
-      <c r="H102" s="30"/>
-      <c r="N102" s="30" t="s">
+      <c r="G102" s="41"/>
+      <c r="H102" s="41"/>
+      <c r="N102" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="O102" s="30"/>
-      <c r="P102" s="30"/>
+      <c r="O102" s="41"/>
+      <c r="P102" s="41"/>
     </row>
     <row r="105" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B105" s="32" t="s">
+      <c r="B105" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="C105" s="32"/>
-      <c r="D105" s="32"/>
-      <c r="F105" s="29" t="s">
+      <c r="C105" s="43"/>
+      <c r="D105" s="43"/>
+      <c r="F105" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="G105" s="29"/>
-      <c r="H105" s="29"/>
-      <c r="J105" s="31" t="s">
+      <c r="G105" s="31"/>
+      <c r="H105" s="31"/>
+      <c r="J105" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="K105" s="31"/>
-      <c r="L105" s="31"/>
-      <c r="N105" s="29" t="s">
+      <c r="K105" s="42"/>
+      <c r="L105" s="42"/>
+      <c r="N105" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="O105" s="29"/>
-      <c r="P105" s="29"/>
+      <c r="O105" s="31"/>
+      <c r="P105" s="31"/>
     </row>
     <row r="106" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B106" s="17" t="s">
@@ -4858,11 +5133,11 @@
         <v>1</v>
       </c>
       <c r="F106" s="21" t="str">
-        <f t="shared" ref="F106:F129" si="20">"_res_." &amp; C106</f>
+        <f ref="F106:F129" si="20" t="shared">"_res_." &amp; C106</f>
         <v>_res_.test</v>
       </c>
       <c r="G106" s="27" t="str">
-        <f t="shared" ref="G106:G131" si="21">C106</f>
+        <f ref="G106:G131" si="21" t="shared">C106</f>
         <v>test</v>
       </c>
       <c r="H106" s="17">
@@ -4878,11 +5153,11 @@
         <v>1</v>
       </c>
       <c r="N106" s="21" t="str">
-        <f t="shared" ref="N106:N129" si="22">"_res_." &amp; K106</f>
+        <f ref="N106:N129" si="22" t="shared">"_res_." &amp; K106</f>
         <v>_res_.test</v>
       </c>
       <c r="O106" s="27" t="str">
-        <f t="shared" ref="O106:O131" si="23">K106</f>
+        <f ref="O106:O131" si="23" t="shared">K106</f>
         <v>test</v>
       </c>
       <c r="P106" s="17">
@@ -4900,11 +5175,11 @@
         <v>2</v>
       </c>
       <c r="F107" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="G107" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>byteValue</v>
       </c>
       <c r="H107" s="13"/>
@@ -4916,11 +5191,11 @@
       </c>
       <c r="L107" s="17"/>
       <c r="N107" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="O107" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>byteValue</v>
       </c>
       <c r="P107" s="13"/>
@@ -4936,11 +5211,11 @@
         <v>2</v>
       </c>
       <c r="F108" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="G108" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="H108" s="13"/>
@@ -4952,11 +5227,11 @@
       </c>
       <c r="L108" s="17"/>
       <c r="N108" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="O108" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="P108" s="13"/>
@@ -4972,11 +5247,11 @@
         <v>2</v>
       </c>
       <c r="F109" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="G109" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="H109" s="13"/>
@@ -4988,11 +5263,11 @@
       </c>
       <c r="L109" s="17"/>
       <c r="N109" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="O109" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="P109" s="13"/>
@@ -5008,11 +5283,11 @@
         <v>2</v>
       </c>
       <c r="F110" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="G110" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="H110" s="13"/>
@@ -5024,11 +5299,11 @@
       </c>
       <c r="L110" s="17"/>
       <c r="N110" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="O110" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="P110" s="13"/>
@@ -5044,11 +5319,11 @@
         <v>2</v>
       </c>
       <c r="F111" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="G111" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="H111" s="13"/>
@@ -5060,11 +5335,11 @@
       </c>
       <c r="L111" s="17"/>
       <c r="N111" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="O111" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="P111" s="13"/>
@@ -5080,11 +5355,11 @@
         <v>2</v>
       </c>
       <c r="F112" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="G112" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="H112" s="13"/>
@@ -5096,11 +5371,11 @@
       </c>
       <c r="L112" s="17"/>
       <c r="N112" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="O112" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="P112" s="13"/>
@@ -5116,11 +5391,11 @@
         <v>2</v>
       </c>
       <c r="F113" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="G113" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="H113" s="13"/>
@@ -5132,11 +5407,11 @@
       </c>
       <c r="L113" s="17"/>
       <c r="N113" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="O113" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="P113" s="13"/>
@@ -5152,11 +5427,11 @@
         <v>2</v>
       </c>
       <c r="F114" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="G114" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="H114" s="13"/>
@@ -5168,11 +5443,11 @@
       </c>
       <c r="L114" s="17"/>
       <c r="N114" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="O114" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="P114" s="13"/>
@@ -5188,11 +5463,11 @@
         <v>2</v>
       </c>
       <c r="F115" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.stringValue</v>
       </c>
       <c r="G115" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>stringValue</v>
       </c>
       <c r="H115" s="13"/>
@@ -5204,11 +5479,11 @@
       </c>
       <c r="L115" s="17"/>
       <c r="N115" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.stringValue</v>
       </c>
       <c r="O115" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>stringValue</v>
       </c>
       <c r="P115" s="13"/>
@@ -5224,11 +5499,11 @@
         <v>2</v>
       </c>
       <c r="F116" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.dateValue</v>
       </c>
       <c r="G116" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>dateValue</v>
       </c>
       <c r="H116" s="2"/>
@@ -5240,11 +5515,11 @@
       </c>
       <c r="L116" s="17"/>
       <c r="N116" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.dateValue</v>
       </c>
       <c r="O116" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>dateValue</v>
       </c>
       <c r="P116" s="2"/>
@@ -5260,11 +5535,11 @@
         <v>2</v>
       </c>
       <c r="F117" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.bigIntValue</v>
       </c>
       <c r="G117" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>bigIntValue</v>
       </c>
       <c r="H117" s="13"/>
@@ -5276,11 +5551,11 @@
       </c>
       <c r="L117" s="17"/>
       <c r="N117" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.bigIntValue</v>
       </c>
       <c r="O117" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>bigIntValue</v>
       </c>
       <c r="P117" s="13"/>
@@ -5296,11 +5571,11 @@
         <v>2</v>
       </c>
       <c r="F118" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.bigDecValue</v>
       </c>
       <c r="G118" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>bigDecValue</v>
       </c>
       <c r="H118" s="13"/>
@@ -5312,11 +5587,11 @@
       </c>
       <c r="L118" s="17"/>
       <c r="N118" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.bigDecValue</v>
       </c>
       <c r="O118" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>bigDecValue</v>
       </c>
       <c r="P118" s="13"/>
@@ -5332,11 +5607,11 @@
         <v>2</v>
       </c>
       <c r="F119" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.colValue</v>
       </c>
       <c r="G119" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>colValue</v>
       </c>
       <c r="H119" s="13"/>
@@ -5348,11 +5623,11 @@
       </c>
       <c r="L119" s="17"/>
       <c r="N119" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.colValue</v>
       </c>
       <c r="O119" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>colValue</v>
       </c>
       <c r="P119" s="13"/>
@@ -5368,11 +5643,11 @@
         <v>2</v>
       </c>
       <c r="F120" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.listValue</v>
       </c>
       <c r="G120" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>listValue</v>
       </c>
       <c r="H120" s="13"/>
@@ -5384,11 +5659,11 @@
       </c>
       <c r="L120" s="17"/>
       <c r="N120" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.listValue</v>
       </c>
       <c r="O120" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>listValue</v>
       </c>
       <c r="P120" s="13"/>
@@ -5404,11 +5679,11 @@
         <v>2</v>
       </c>
       <c r="F121" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.mapValue</v>
       </c>
       <c r="G121" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>mapValue</v>
       </c>
       <c r="H121" s="13"/>
@@ -5420,11 +5695,11 @@
       </c>
       <c r="L121" s="17"/>
       <c r="N121" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.mapValue</v>
       </c>
       <c r="O121" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>mapValue</v>
       </c>
       <c r="P121" s="13"/>
@@ -5440,11 +5715,11 @@
         <v>2</v>
       </c>
       <c r="F122" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.setValue</v>
       </c>
       <c r="G122" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>setValue</v>
       </c>
       <c r="H122" s="13"/>
@@ -5456,11 +5731,11 @@
       </c>
       <c r="L122" s="17"/>
       <c r="N122" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.setValue</v>
       </c>
       <c r="O122" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>setValue</v>
       </c>
       <c r="P122" s="13"/>
@@ -5476,11 +5751,11 @@
         <v>2</v>
       </c>
       <c r="F123" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.arrayList</v>
       </c>
       <c r="G123" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>arrayList</v>
       </c>
       <c r="H123" s="21"/>
@@ -5492,11 +5767,11 @@
       </c>
       <c r="L123" s="21"/>
       <c r="N123" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.arrayList</v>
       </c>
       <c r="O123" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>arrayList</v>
       </c>
       <c r="P123" s="21"/>
@@ -5512,11 +5787,11 @@
         <v>2</v>
       </c>
       <c r="F124" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.hashMap</v>
       </c>
       <c r="G124" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>hashMap</v>
       </c>
       <c r="H124" s="21"/>
@@ -5528,11 +5803,11 @@
       </c>
       <c r="L124" s="21"/>
       <c r="N124" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.hashMap</v>
       </c>
       <c r="O124" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>hashMap</v>
       </c>
       <c r="P124" s="21"/>
@@ -5548,11 +5823,11 @@
         <v>2</v>
       </c>
       <c r="F125" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.hashSet</v>
       </c>
       <c r="G125" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>hashSet</v>
       </c>
       <c r="H125" s="21"/>
@@ -5564,11 +5839,11 @@
       </c>
       <c r="L125" s="21"/>
       <c r="N125" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.hashSet</v>
       </c>
       <c r="O125" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>hashSet</v>
       </c>
       <c r="P125" s="21"/>
@@ -5584,11 +5859,11 @@
         <v>2</v>
       </c>
       <c r="F126" s="22" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.gender</v>
       </c>
       <c r="G126" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>gender</v>
       </c>
       <c r="H126" s="22"/>
@@ -5600,11 +5875,11 @@
       </c>
       <c r="L126" s="22"/>
       <c r="N126" s="22" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.gender</v>
       </c>
       <c r="O126" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>gender</v>
       </c>
       <c r="P126" s="22"/>
@@ -5620,11 +5895,11 @@
         <v>2</v>
       </c>
       <c r="F127" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.address</v>
       </c>
       <c r="G127" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>address</v>
       </c>
       <c r="H127" s="20"/>
@@ -5636,11 +5911,11 @@
       </c>
       <c r="L127" s="20"/>
       <c r="N127" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.address</v>
       </c>
       <c r="O127" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>address</v>
       </c>
       <c r="P127" s="20"/>
@@ -5656,11 +5931,11 @@
         <v>2</v>
       </c>
       <c r="F128" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.person</v>
       </c>
       <c r="G128" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>person</v>
       </c>
       <c r="H128" s="20"/>
@@ -5672,11 +5947,11 @@
       </c>
       <c r="L128" s="20"/>
       <c r="N128" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.person</v>
       </c>
       <c r="O128" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>person</v>
       </c>
       <c r="P128" s="20"/>
@@ -5692,11 +5967,11 @@
         <v>2</v>
       </c>
       <c r="F129" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f si="20" t="shared"/>
         <v>_res_.auto</v>
       </c>
       <c r="G129" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>auto</v>
       </c>
       <c r="H129" s="20"/>
@@ -5708,11 +5983,11 @@
       </c>
       <c r="L129" s="20"/>
       <c r="N129" s="21" t="str">
-        <f t="shared" si="22"/>
+        <f si="22" t="shared"/>
         <v>_res_.auto</v>
       </c>
       <c r="O129" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>auto</v>
       </c>
       <c r="P129" s="20"/>
@@ -5732,7 +6007,7 @@
         <v>_res_.roudingMode</v>
       </c>
       <c r="G130" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>roudingMode</v>
       </c>
       <c r="H130" s="25"/>
@@ -5748,7 +6023,7 @@
         <v>_res_.roudingMode</v>
       </c>
       <c r="O130" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>roudingMode</v>
       </c>
       <c r="P130" s="25"/>
@@ -5764,11 +6039,11 @@
         <v>2</v>
       </c>
       <c r="F131" s="26" t="str">
-        <f t="shared" ref="F131" si="24">"_res_." &amp; C131</f>
+        <f ref="F131" si="24" t="shared">"_res_." &amp; C131</f>
         <v>_res_.dv</v>
       </c>
       <c r="G131" s="27" t="str">
-        <f t="shared" si="21"/>
+        <f si="21" t="shared"/>
         <v>dv</v>
       </c>
       <c r="H131" s="2"/>
@@ -5780,60 +6055,60 @@
       </c>
       <c r="L131" s="26"/>
       <c r="N131" s="26" t="str">
-        <f t="shared" ref="N131" si="25">"_res_." &amp; K131</f>
+        <f ref="N131" si="25" t="shared">"_res_." &amp; K131</f>
         <v>_res_.dv</v>
       </c>
       <c r="O131" s="27" t="str">
-        <f t="shared" si="23"/>
+        <f si="23" t="shared"/>
         <v>dv</v>
       </c>
       <c r="P131" s="26"/>
     </row>
     <row r="134" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F134" s="29" t="s">
+      <c r="F134" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="G134" s="29"/>
-      <c r="H134" s="29"/>
-      <c r="N134" s="29" t="s">
+      <c r="G134" s="31"/>
+      <c r="H134" s="31"/>
+      <c r="N134" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="O134" s="29"/>
-      <c r="P134" s="29"/>
+      <c r="O134" s="31"/>
+      <c r="P134" s="31"/>
     </row>
     <row r="135" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F135" s="30" t="s">
+      <c r="F135" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="G135" s="30"/>
-      <c r="H135" s="30"/>
-      <c r="N135" s="30" t="s">
+      <c r="G135" s="41"/>
+      <c r="H135" s="41"/>
+      <c r="N135" s="41" t="s">
         <v>172</v>
       </c>
-      <c r="O135" s="30"/>
-      <c r="P135" s="30"/>
+      <c r="O135" s="41"/>
+      <c r="P135" s="41"/>
     </row>
     <row r="138" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B138" s="32" t="s">
+      <c r="B138" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="C138" s="32"/>
-      <c r="D138" s="32"/>
-      <c r="F138" s="33" t="s">
+      <c r="C138" s="43"/>
+      <c r="D138" s="43"/>
+      <c r="F138" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="G138" s="33"/>
-      <c r="H138" s="33"/>
-      <c r="J138" s="31" t="s">
+      <c r="G138" s="44"/>
+      <c r="H138" s="44"/>
+      <c r="J138" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="K138" s="31"/>
-      <c r="L138" s="31"/>
-      <c r="N138" s="33" t="s">
+      <c r="K138" s="42"/>
+      <c r="L138" s="42"/>
+      <c r="N138" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="O138" s="33"/>
-      <c r="P138" s="33"/>
+      <c r="O138" s="44"/>
+      <c r="P138" s="44"/>
     </row>
     <row r="139" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B139" s="17" t="s">
@@ -5846,11 +6121,11 @@
         <v>1</v>
       </c>
       <c r="F139" s="21" t="str">
-        <f t="shared" ref="F139:F147" si="26">"_res_." &amp; C139</f>
+        <f ref="F139:F147" si="26" t="shared">"_res_." &amp; C139</f>
         <v>_res_.test</v>
       </c>
       <c r="G139" s="27" t="str">
-        <f t="shared" ref="G139:G147" si="27">C139</f>
+        <f ref="G139:G147" si="27" t="shared">C139</f>
         <v>test</v>
       </c>
       <c r="H139" s="17">
@@ -5866,11 +6141,11 @@
         <v>1</v>
       </c>
       <c r="N139" s="21" t="str">
-        <f t="shared" ref="N139:N147" si="28">"_res_." &amp; K139</f>
+        <f ref="N139:N147" si="28" t="shared">"_res_." &amp; K139</f>
         <v>_res_.test</v>
       </c>
       <c r="O139" s="27" t="str">
-        <f t="shared" ref="O139:O147" si="29">K139</f>
+        <f ref="O139:O147" si="29" t="shared">K139</f>
         <v>test</v>
       </c>
       <c r="P139" s="17">
@@ -5888,11 +6163,11 @@
         <v>2</v>
       </c>
       <c r="F140" s="21" t="str">
-        <f t="shared" si="26"/>
+        <f si="26" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="G140" s="27" t="str">
-        <f t="shared" si="27"/>
+        <f si="27" t="shared"/>
         <v>byteValue</v>
       </c>
       <c r="H140" s="13"/>
@@ -5904,11 +6179,11 @@
       </c>
       <c r="L140" s="17"/>
       <c r="N140" s="21" t="str">
-        <f t="shared" si="28"/>
+        <f si="28" t="shared"/>
         <v>_res_.byteValue</v>
       </c>
       <c r="O140" s="27" t="str">
-        <f t="shared" si="29"/>
+        <f si="29" t="shared"/>
         <v>byteValue</v>
       </c>
       <c r="P140" s="13"/>
@@ -5924,11 +6199,11 @@
         <v>2</v>
       </c>
       <c r="F141" s="21" t="str">
-        <f t="shared" si="26"/>
+        <f si="26" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="G141" s="27" t="str">
-        <f t="shared" si="27"/>
+        <f si="27" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="H141" s="13"/>
@@ -5940,11 +6215,11 @@
       </c>
       <c r="L141" s="17"/>
       <c r="N141" s="21" t="str">
-        <f t="shared" si="28"/>
+        <f si="28" t="shared"/>
         <v>_res_.shortValue</v>
       </c>
       <c r="O141" s="27" t="str">
-        <f t="shared" si="29"/>
+        <f si="29" t="shared"/>
         <v>shortValue</v>
       </c>
       <c r="P141" s="13"/>
@@ -5960,11 +6235,11 @@
         <v>2</v>
       </c>
       <c r="F142" s="21" t="str">
-        <f t="shared" si="26"/>
+        <f si="26" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="G142" s="27" t="str">
-        <f t="shared" si="27"/>
+        <f si="27" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="H142" s="13"/>
@@ -5976,11 +6251,11 @@
       </c>
       <c r="L142" s="17"/>
       <c r="N142" s="21" t="str">
-        <f t="shared" si="28"/>
+        <f si="28" t="shared"/>
         <v>_res_.intValue</v>
       </c>
       <c r="O142" s="27" t="str">
-        <f t="shared" si="29"/>
+        <f si="29" t="shared"/>
         <v>intValue</v>
       </c>
       <c r="P142" s="13"/>
@@ -5996,11 +6271,11 @@
         <v>2</v>
       </c>
       <c r="F143" s="21" t="str">
-        <f t="shared" si="26"/>
+        <f si="26" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="G143" s="27" t="str">
-        <f t="shared" si="27"/>
+        <f si="27" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="H143" s="13"/>
@@ -6012,11 +6287,11 @@
       </c>
       <c r="L143" s="17"/>
       <c r="N143" s="21" t="str">
-        <f t="shared" si="28"/>
+        <f si="28" t="shared"/>
         <v>_res_.longValue</v>
       </c>
       <c r="O143" s="27" t="str">
-        <f t="shared" si="29"/>
+        <f si="29" t="shared"/>
         <v>longValue</v>
       </c>
       <c r="P143" s="13"/>
@@ -6032,11 +6307,11 @@
         <v>2</v>
       </c>
       <c r="F144" s="21" t="str">
-        <f t="shared" si="26"/>
+        <f si="26" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="G144" s="27" t="str">
-        <f t="shared" si="27"/>
+        <f si="27" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="H144" s="13"/>
@@ -6048,11 +6323,11 @@
       </c>
       <c r="L144" s="17"/>
       <c r="N144" s="21" t="str">
-        <f t="shared" si="28"/>
+        <f si="28" t="shared"/>
         <v>_res_.floatValue</v>
       </c>
       <c r="O144" s="27" t="str">
-        <f t="shared" si="29"/>
+        <f si="29" t="shared"/>
         <v>floatValue</v>
       </c>
       <c r="P144" s="13"/>
@@ -6068,11 +6343,11 @@
         <v>2</v>
       </c>
       <c r="F145" s="21" t="str">
-        <f t="shared" si="26"/>
+        <f si="26" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="G145" s="27" t="str">
-        <f t="shared" si="27"/>
+        <f si="27" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="H145" s="13"/>
@@ -6084,11 +6359,11 @@
       </c>
       <c r="L145" s="17"/>
       <c r="N145" s="21" t="str">
-        <f t="shared" si="28"/>
+        <f si="28" t="shared"/>
         <v>_res_.doubleValue</v>
       </c>
       <c r="O145" s="27" t="str">
-        <f t="shared" si="29"/>
+        <f si="29" t="shared"/>
         <v>doubleValue</v>
       </c>
       <c r="P145" s="13"/>
@@ -6104,11 +6379,11 @@
         <v>2</v>
       </c>
       <c r="F146" s="21" t="str">
-        <f t="shared" si="26"/>
+        <f si="26" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="G146" s="27" t="str">
-        <f t="shared" si="27"/>
+        <f si="27" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="H146" s="13"/>
@@ -6120,11 +6395,11 @@
       </c>
       <c r="L146" s="17"/>
       <c r="N146" s="21" t="str">
-        <f t="shared" si="28"/>
+        <f si="28" t="shared"/>
         <v>_res_.booleanValue</v>
       </c>
       <c r="O146" s="27" t="str">
-        <f t="shared" si="29"/>
+        <f si="29" t="shared"/>
         <v>booleanValue</v>
       </c>
       <c r="P146" s="13"/>
@@ -6140,11 +6415,11 @@
         <v>2</v>
       </c>
       <c r="F147" s="21" t="str">
-        <f t="shared" si="26"/>
+        <f si="26" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="G147" s="27" t="str">
-        <f t="shared" si="27"/>
+        <f si="27" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="H147" s="13"/>
@@ -6156,49 +6431,92 @@
       </c>
       <c r="L147" s="17"/>
       <c r="N147" s="21" t="str">
-        <f t="shared" si="28"/>
+        <f si="28" t="shared"/>
         <v>_res_.charValue</v>
       </c>
       <c r="O147" s="27" t="str">
-        <f t="shared" si="29"/>
+        <f si="29" t="shared"/>
         <v>charValue</v>
       </c>
       <c r="P147" s="13"/>
     </row>
     <row r="151" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B151" s="29" t="s">
+      <c r="B151" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C151" s="29"/>
-      <c r="D151" s="29"/>
+      <c r="C151" s="31"/>
+      <c r="D151" s="31"/>
+      <c r="F151" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="G151" s="31"/>
+      <c r="H151" s="31"/>
+      <c r="J151" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="K151" s="31"/>
+      <c r="L151" s="31"/>
     </row>
     <row r="152" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B152" s="45" t="s">
+      <c r="B152" s="56" t="s">
         <v>242</v>
       </c>
-      <c r="C152" s="46"/>
-      <c r="D152" s="47"/>
+      <c r="C152" s="57"/>
+      <c r="D152" s="58"/>
+      <c r="F152" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="G152" s="33"/>
+      <c r="H152" s="34"/>
+      <c r="J152" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="K152" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="L152" s="2" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="153" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B153" s="45" t="s">
+      <c r="B153" s="56" t="s">
         <v>243</v>
       </c>
-      <c r="C153" s="46"/>
-      <c r="D153" s="47"/>
+      <c r="C153" s="57"/>
+      <c r="D153" s="58"/>
+      <c r="F153" s="35"/>
+      <c r="G153" s="36"/>
+      <c r="H153" s="37"/>
     </row>
     <row r="154" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B154" s="45" t="s">
+      <c r="B154" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="C154" s="46"/>
-      <c r="D154" s="47"/>
+      <c r="C154" s="57"/>
+      <c r="D154" s="58"/>
+      <c r="F154" s="35"/>
+      <c r="G154" s="36"/>
+      <c r="H154" s="37"/>
+    </row>
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F155" s="35"/>
+      <c r="G155" s="36"/>
+      <c r="H155" s="37"/>
+    </row>
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F156" s="35"/>
+      <c r="G156" s="36"/>
+      <c r="H156" s="37"/>
     </row>
     <row r="157" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B157" s="29" t="s">
+      <c r="B157" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="C157" s="29"/>
-      <c r="D157" s="29"/>
+      <c r="C157" s="31"/>
+      <c r="D157" s="31"/>
+      <c r="F157" s="35"/>
+      <c r="G157" s="36"/>
+      <c r="H157" s="37"/>
     </row>
     <row r="158" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="s">
@@ -6210,6 +6528,9 @@
       <c r="D158" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="F158" s="35"/>
+      <c r="G158" s="36"/>
+      <c r="H158" s="37"/>
     </row>
     <row r="159" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
@@ -6219,6 +6540,9 @@
         <v>209</v>
       </c>
       <c r="D159" s="1"/>
+      <c r="F159" s="35"/>
+      <c r="G159" s="36"/>
+      <c r="H159" s="37"/>
     </row>
     <row r="160" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B160" s="1" t="s">
@@ -6228,15 +6552,31 @@
         <v>210</v>
       </c>
       <c r="D160" s="1"/>
-    </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B163" s="29" t="s">
+      <c r="F160" s="35"/>
+      <c r="G160" s="36"/>
+      <c r="H160" s="37"/>
+    </row>
+    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F161" s="35"/>
+      <c r="G161" s="36"/>
+      <c r="H161" s="37"/>
+    </row>
+    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F162" s="35"/>
+      <c r="G162" s="36"/>
+      <c r="H162" s="37"/>
+    </row>
+    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B163" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="C163" s="29"/>
-      <c r="D163" s="29"/>
-    </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C163" s="31"/>
+      <c r="D163" s="31"/>
+      <c r="F163" s="38"/>
+      <c r="G163" s="39"/>
+      <c r="H163" s="40"/>
+    </row>
+    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B164" s="23" t="s">
         <v>0</v>
       </c>
@@ -6247,7 +6587,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="s">
         <v>4</v>
       </c>
@@ -6256,7 +6596,7 @@
       </c>
       <c r="D165" s="1"/>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="s">
         <v>6</v>
       </c>
@@ -6267,14 +6607,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B169" s="29" t="s">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B169" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="C169" s="29"/>
-      <c r="D169" s="29"/>
-    </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C169" s="31"/>
+      <c r="D169" s="31"/>
+    </row>
+    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
         <v>8</v>
       </c>
@@ -6285,7 +6625,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="s">
         <v>212</v>
       </c>
@@ -6296,7 +6636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="s">
         <v>6</v>
       </c>
@@ -6305,72 +6645,211 @@
       </c>
       <c r="D172" s="1"/>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B175" s="31" t="s">
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B175" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="C175" s="31"/>
-      <c r="D175" s="31"/>
-      <c r="E175" s="31"/>
-      <c r="F175" s="31"/>
-    </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C175" s="42"/>
+      <c r="D175" s="42"/>
+      <c r="E175" s="42"/>
+      <c r="F175" s="42"/>
+    </row>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C176" s="39" t="s">
+      <c r="C176" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="D176" s="40"/>
-      <c r="E176" s="40"/>
-      <c r="F176" s="41"/>
+      <c r="D176" s="51"/>
+      <c r="E176" s="51"/>
+      <c r="F176" s="52"/>
     </row>
     <row r="177" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B177" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C177" s="42" t="s">
+      <c r="C177" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="D177" s="43"/>
-      <c r="E177" s="43"/>
-      <c r="F177" s="44"/>
+      <c r="D177" s="54"/>
+      <c r="E177" s="54"/>
+      <c r="F177" s="55"/>
     </row>
     <row r="178" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B178" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C178" s="38" t="s">
+      <c r="C178" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D178" s="35"/>
-      <c r="E178" s="35"/>
-      <c r="F178" s="36"/>
+      <c r="D178" s="46"/>
+      <c r="E178" s="46"/>
+      <c r="F178" s="47"/>
     </row>
     <row r="179" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B179" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C179" s="37" t="s">
+      <c r="C179" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="D179" s="37"/>
-      <c r="E179" s="37"/>
-      <c r="F179" s="37"/>
+      <c r="D179" s="48"/>
+      <c r="E179" s="48"/>
+      <c r="F179" s="48"/>
     </row>
     <row r="180" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B180" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C180" s="34" t="s">
+      <c r="C180" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="D180" s="35"/>
-      <c r="E180" s="35"/>
-      <c r="F180" s="36"/>
+      <c r="D180" s="46"/>
+      <c r="E180" s="46"/>
+      <c r="F180" s="47"/>
+    </row>
+    <row r="182">
+      <c r="B182" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="C182" s="31"/>
+      <c r="D182" s="31"/>
+    </row>
+    <row r="183">
+      <c r="B183" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="C183" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="D183" s="34" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="B184" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C184" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D184" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="B185" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C185" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D185" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="B186" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C186" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D186" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="B187" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C187" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D187" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="B188" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C188" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D188" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C189" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D189" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="B190" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C190" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D190" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="B191" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C191" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D191" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="B192" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C192" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D192" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="B193" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C193" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D193" s="37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="B194" s="38" t="s">
+        <v>264</v>
+      </c>
+      <c r="C194" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="D194" s="40" t="s">
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="61">
+  <mergeCells count="64">
     <mergeCell ref="B151:D151"/>
     <mergeCell ref="B152:D152"/>
     <mergeCell ref="B153:D153"/>
@@ -6378,13 +6857,7 @@
     <mergeCell ref="F105:H105"/>
     <mergeCell ref="B138:D138"/>
     <mergeCell ref="B105:D105"/>
-    <mergeCell ref="N134:P134"/>
-    <mergeCell ref="N135:P135"/>
-    <mergeCell ref="N138:P138"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="J138:L138"/>
+    <mergeCell ref="F151:H151"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="N7:P7"/>
@@ -6426,22 +6899,33 @@
     <mergeCell ref="N89:P89"/>
     <mergeCell ref="N40:P40"/>
     <mergeCell ref="F86:H86"/>
+    <mergeCell ref="J151:L151"/>
+    <mergeCell ref="F152:H163"/>
     <mergeCell ref="N101:P101"/>
     <mergeCell ref="N102:P102"/>
     <mergeCell ref="N105:P105"/>
     <mergeCell ref="F101:H101"/>
     <mergeCell ref="F102:H102"/>
     <mergeCell ref="J105:L105"/>
+    <mergeCell ref="N134:P134"/>
+    <mergeCell ref="N135:P135"/>
+    <mergeCell ref="N138:P138"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="J138:L138"/>
+    <mergeCell ref="B182:D182"/>
+    <mergeCell ref="B183:D194"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -6449,25 +6933,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -6786,15 +7270,15 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
@@ -6858,13 +7342,13 @@
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B20:H20"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
@@ -6872,15 +7356,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="48"/>
+      <c r="C3" s="59"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
@@ -6902,6 +7386,6 @@
   <mergeCells count="1">
     <mergeCell ref="B3:C3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>